<commit_message>
feat: update playlist and session management, add new tracks, and improve user interface
</commit_message>
<xml_diff>
--- a/mi_playlist_seleccionada.xlsx
+++ b/mi_playlist_seleccionada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,238 +453,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>RAMONCITO</t>
+          <t>EL SABOR DE NACHO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SI TU NO, LA OTRA</t>
+          <t>QUE SE SEPA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>00:03:10</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TITO RAMIREZ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>POWWER OF LOVE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>00:03:40</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>TITO RAMIREZ</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>HAVE TO SEE MA BABE</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>00:03:18</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>CELIA, JOHNNY, JUSTO &amp; PAPO</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>BESITO DE COCO</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>00:04:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>CELIA, JOHNNY, JUSTO &amp; PAPO</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>GUILLATE</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>00:05:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>ROMPERAYO</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>QUE TUMBA</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>00:03:15</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ROMPERAYO</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>HEY, NO TE FAJES</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>00:03:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>LOS FULANOS</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>BLUE MONDAY</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>00:03:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>LOS FULANOS</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>WHY DON'T WE DO SOME BOOGALOO</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>00:03:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>VIVA ZEQUEIRA</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>CHICA BOUM2:49</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>00:02:49</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>BOOGALOO ASSASSINS</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>NO NO NO</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>00:03:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>BOOGALOO ASSASSINS</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>EVIL WAYS (INSTRUMENTAL)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>00:02:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>LUCHITO</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>THE HARLEM BUGALÚ</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
           <t>00:03:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>JOAQUIN MARQUEZ</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>MALA MANIA</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>00:03:40</t>
         </is>
       </c>
     </row>

</xml_diff>